<commit_message>
[1.1.2.0] quarter to month update
</commit_message>
<xml_diff>
--- a/IRCS2_build/Input Sheet.xlsx
+++ b/IRCS2_build/Input Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. IRCS Automation\Control 2 DEV\IRCS-v2\IRCS2_build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59456CFC-132D-4BAC-8A83-A4B40D99AF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2E638D-13B3-4498-A065-EC3D4554BB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1CB29936-90A1-4B24-80D1-9DB6A66D7875}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">UL!$A$1:$B$151</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="496">
   <si>
     <t>Prophet Code</t>
   </si>
@@ -1507,9 +1507,6 @@
     <t>D:\1. IRCS Automation\Source\IRCS2\LGC &amp; LGM Campaign\RESERVE_TRADSHA_RWNB_IFRS_20250402.txt</t>
   </si>
   <si>
-    <t>Reporting Quarter</t>
-  </si>
-  <si>
     <t>Financial Year</t>
   </si>
   <si>
@@ -1535,6 +1532,9 @@
   </si>
   <si>
     <t>D:\1. IRCS Automation\Control 2 DEV\IRCS-v2\IRCS2_build\source\Summary.csv</t>
+  </si>
+  <si>
+    <t>Reporting Month</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2104,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2119,6 +2119,7 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2497,7 +2498,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,15 +2517,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="B2" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B3" s="9">
         <v>2025</v>
@@ -2535,7 +2536,7 @@
         <v>450</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2543,7 +2544,7 @@
         <v>451</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2551,7 +2552,7 @@
         <v>453</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2559,7 +2560,7 @@
         <v>452</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2567,7 +2568,7 @@
         <v>479</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2588,7 +2589,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>484</v>
@@ -2596,7 +2597,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>485</v>
@@ -2607,7 +2608,7 @@
         <v>454</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -2622,7 +2623,9 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2634,48 +2637,40 @@
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>486</v>
-      </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>487</v>
-      </c>
-      <c r="B3" s="9">
-        <v>2025</v>
-      </c>
+      <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
+      <c r="B5" s="12"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
+      <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
+      <c r="B10" s="12"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
+      <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
+      <c r="B13" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>